<commit_message>
Added mp results to diploma
</commit_message>
<xml_diff>
--- a/example/mp_reports_01KP_26.05.2018-1.31.6.883_50_items/strongly_correled_50.xlsx
+++ b/example/mp_reports_01KP_26.05.2018-1.31.6.883_50_items/strongly_correled_50.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>Elapsed Time (ms)</t>
   </si>
@@ -126,10 +126,13 @@
     <t>GA deviation</t>
   </si>
   <si>
-    <t xml:space="preserve"> max deviation</t>
-  </si>
-  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>GA avg deviation</t>
+  </si>
+  <si>
+    <t>GA max deviation</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
         <v>2254.5</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>4321.5</v>
@@ -598,7 +601,7 @@
         <v>1088.5</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>4326.5</v>
@@ -654,7 +657,7 @@
         <v>3014.5</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>4330.5</v>
@@ -710,7 +713,7 @@
         <v>8407</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>4318</v>
@@ -766,7 +769,7 @@
         <v>2323.5</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>4306</v>
@@ -822,7 +825,7 @@
         <v>4648.5</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>4345</v>
@@ -878,7 +881,7 @@
         <v>9516.5</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>4338.5</v>
@@ -934,7 +937,7 @@
         <v>5868.5</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10">
         <v>4285</v>
@@ -990,7 +993,7 @@
         <v>7517</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <v>4321</v>
@@ -1046,7 +1049,7 @@
         <v>2405</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>4341.5</v>
@@ -1102,7 +1105,7 @@
         <v>16598</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>4356</v>
@@ -1158,7 +1161,7 @@
         <v>3202</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <v>4366</v>
@@ -1214,7 +1217,7 @@
         <v>4135</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15">
         <v>4364</v>
@@ -1270,7 +1273,7 @@
         <v>2749</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16">
         <v>4396.5</v>
@@ -1326,7 +1329,7 @@
         <v>3945.5</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17">
         <v>4354</v>
@@ -1382,7 +1385,7 @@
         <v>1282</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18">
         <v>4402</v>
@@ -1438,7 +1441,7 @@
         <v>4570.5</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19">
         <v>4341</v>
@@ -1494,7 +1497,7 @@
         <v>4276</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20">
         <v>4400</v>
@@ -1550,7 +1553,7 @@
         <v>6102</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21">
         <v>4410.5</v>
@@ -1606,7 +1609,7 @@
         <v>5336</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22">
         <v>4395.5</v>
@@ -1662,7 +1665,7 @@
         <v>2370</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23">
         <v>4356</v>
@@ -1718,7 +1721,7 @@
         <v>4611.5</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24">
         <v>4370</v>
@@ -1774,7 +1777,7 @@
         <v>1149.5</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25">
         <v>4404.5</v>
@@ -1830,7 +1833,7 @@
         <v>1244</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26">
         <v>4419</v>
@@ -1886,7 +1889,7 @@
         <v>17606</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27">
         <v>4402.5</v>
@@ -1942,7 +1945,7 @@
         <v>1759.5</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>4387.5</v>
@@ -1998,7 +2001,7 @@
         <v>2232.5</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F29">
         <v>4403</v>
@@ -2054,7 +2057,7 @@
         <v>2515.5</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30">
         <v>4397</v>
@@ -2110,7 +2113,7 @@
         <v>541.5</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F31">
         <v>4381</v>
@@ -2166,7 +2169,7 @@
         <v>2756.5</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F32">
         <v>4383.5</v>
@@ -2275,20 +2278,26 @@
         <v>21</v>
       </c>
       <c r="B42" s="1">
+        <f>($B$33-COUNTIF($Q$3:$Q$32,0))/$B$33</f>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>3.0240110000000001E-3</v>
+      <c r="A44" s="1">
+        <f>AVERAGE(Q3:Q32)</f>
+        <v>2.0757304750576534E-3</v>
+      </c>
+      <c r="B44" s="1">
+        <f>MAX(Q3:Q32)</f>
+        <v>3.024010503722419E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added conclusions about MP experiments
</commit_message>
<xml_diff>
--- a/example/mp_reports_01KP_26.05.2018-1.31.6.883_50_items/strongly_correled_50.xlsx
+++ b/example/mp_reports_01KP_26.05.2018-1.31.6.883_50_items/strongly_correled_50.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Elapsed Time (ms)</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>GA max deviation</t>
+  </si>
+  <si>
+    <t>min elapsed time</t>
   </si>
 </sst>
 </file>
@@ -470,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2213,7 @@
         <v>3.024010503722419E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2218,25 +2221,32 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>AVERAGE(G3:G32)</f>
+        <v>54.56666666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2244,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2252,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2260,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2268,12 +2278,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2282,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -2290,7 +2300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f>AVERAGE(Q3:Q32)</f>
         <v>2.0757304750576534E-3</v>

</xml_diff>